<commit_message>
Changes for screen one has been implemented
</commit_message>
<xml_diff>
--- a/src/test/resources/MasterData.xlsx
+++ b/src/test/resources/MasterData.xlsx
@@ -5,12 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="JourneyScreenOneforIndain" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="JourneyScreenOneforNRI" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="JourneyScreenTwo" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="VerifyOTP" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -60,24 +62,136 @@
     <t xml:space="preserve">669228772880</t>
   </si>
   <si>
+    <t xml:space="preserve">CEZPK2904p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9873901989</t>
+  </si>
+  <si>
+    <t xml:space="preserve">navneet@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98760987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">669238226887</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEZPK2879k</t>
+  </si>
+  <si>
     <t xml:space="preserve">CEZPK29019</t>
   </si>
   <si>
-    <t xml:space="preserve">9873901989</t>
-  </si>
-  <si>
-    <t xml:space="preserve">navneet@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">98760987</t>
+    <t xml:space="preserve">firstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dateOfBirth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">houseNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">road/area/sector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">villageTown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pincode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alternateMobileNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestFirstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestLastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14/08/1996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestHoseNo/AptName/Society</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestRoad/Area/Sec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestVillage/Town</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9999999999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digit 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digit 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digit 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digit 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digit 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digit 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -156,7 +270,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -171,6 +285,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -255,16 +377,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.43"/>
@@ -305,9 +427,27 @@
         <v>15</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="navneet@gmail.com"/>
+    <hyperlink ref="D3" r:id="rId2" display="navneet@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -326,11 +466,14 @@
   </sheetPr>
   <dimension ref="D1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1" s="3" t="s">
@@ -354,7 +497,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>13</v>
@@ -378,4 +521,176 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="7" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
sprint 6 test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/MasterData.xlsx
+++ b/src/test/resources/MasterData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,7 @@
     <sheet name="JourneyScreenOneforNRI" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="JourneyScreenTwo" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="VerifyOTP" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="JourneyScreenThree" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -183,6 +184,24 @@
   </si>
   <si>
     <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Father Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mother Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr. N. K. Gupta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mrs. M K. Gupta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100000000</t>
   </si>
 </sst>
 </file>
@@ -379,7 +398,7 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -531,7 +550,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -693,4 +712,54 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.33"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
first stable commit for browser stack
</commit_message>
<xml_diff>
--- a/src/test/resources/MasterData.xlsx
+++ b/src/test/resources/MasterData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="743" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -12,8 +12,13 @@
     <sheet name="JourneyScreenOneforNRI" sheetId="3" r:id="rId3"/>
     <sheet name="JourneyScreenTwo" sheetId="4" r:id="rId4"/>
     <sheet name="JourneyScreenThree" sheetId="5" r:id="rId5"/>
+    <sheet name="dropDownList" sheetId="6" r:id="rId6"/>
+    <sheet name="ErrorMsgValidationSTP-MIAP-WLS" sheetId="7" r:id="rId7"/>
+    <sheet name="ErrorMsgValidationSAP" sheetId="8" r:id="rId8"/>
+    <sheet name="MultipleDataValidationForFTSP" sheetId="9" r:id="rId9"/>
+    <sheet name="personalDetailsSectionValid" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="212">
   <si>
     <t>username</t>
   </si>
@@ -106,45 +111,27 @@
     <t>positiveValidation</t>
   </si>
   <si>
-    <t>TestNegativeValidationqwertyuioplkjhgfdsazxcvbnmmnbvcxzzqwertyuioplkjhgmnbvzx</t>
-  </si>
-  <si>
     <t>negativeValidation</t>
   </si>
   <si>
     <t>TestNegativeValidationqwertyuioplkjhgfdsazxcvbnmmnbvcxzzqwertyuiaoplkjhgmnbvzx</t>
   </si>
   <si>
-    <t>111111UUUUU</t>
-  </si>
-  <si>
     <t>Ifc</t>
   </si>
   <si>
     <t>micr</t>
   </si>
   <si>
-    <t>222UA222233</t>
-  </si>
-  <si>
-    <t>1111111111111111111111111111111111111111111111WWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWW@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@@</t>
-  </si>
-  <si>
     <t>bankName/bankBranch</t>
   </si>
   <si>
     <t>bankAccountNumber</t>
   </si>
   <si>
-    <t>111111111111111E11111111111111111111</t>
-  </si>
-  <si>
     <t>accountHolderName</t>
   </si>
   <si>
-    <t>A.11111111AAAAAAAAAAAAAAAAAAAAAAA</t>
-  </si>
-  <si>
     <t>CEZPK29019#</t>
   </si>
   <si>
@@ -157,35 +144,543 @@
     <t>CPYPP4048C@</t>
   </si>
   <si>
-    <t>TestFirstName1#wwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwww</t>
-  </si>
-  <si>
-    <t>TestLastName1#wwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwww</t>
-  </si>
-  <si>
-    <t>TestHouseQQQ1!QQQQQQQQQQQQQQQQQQQQQQQQQQQQ!1QQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQ</t>
-  </si>
-  <si>
-    <t>TestRoad1!QQQQQQQQQQQQQQQQQQQQQQQQQQQQ!1QQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQQWWWWWWWWWWWWWWWWWWWWWWW</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>11@A1111</t>
   </si>
   <si>
+    <t>passportNumber</t>
+  </si>
+  <si>
+    <t>A12 345671111111@1111</t>
+  </si>
+  <si>
+    <t>passportIssuingCountry</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>isdCode</t>
+  </si>
+  <si>
+    <t>issurersName</t>
+  </si>
+  <si>
+    <t>AXIS Bank</t>
+  </si>
+  <si>
     <t>99A@99999999</t>
+  </si>
+  <si>
+    <t>sumAssured</t>
+  </si>
+  <si>
+    <t>premiumCommitment</t>
+  </si>
+  <si>
+    <t>desiredAnnualIncome</t>
+  </si>
+  <si>
+    <t>annualIncome</t>
+  </si>
+  <si>
+    <t>premiumCommitmentSAP</t>
+  </si>
+  <si>
+    <t>Fund</t>
+  </si>
+  <si>
+    <t>erroMessage</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>500000</t>
+  </si>
+  <si>
+    <t>600000</t>
+  </si>
+  <si>
+    <t>Apartment! 1 Sub-building name
+The Jam Works Building name
+49–51 Fleet Street Street number and street
+LIVERPOOL
+L1 4AR</t>
+  </si>
+  <si>
+    <t>Adolph Blaine#1@ Charles David Earl Frederick Gerald Hubert Irvim John Kenneth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aadhaar
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passport
+</t>
+  </si>
+  <si>
+    <t>PAN Card</t>
+  </si>
+  <si>
+    <t>Driving License</t>
+  </si>
+  <si>
+    <t>Voter ID</t>
+  </si>
+  <si>
+    <t>State/Central Govt. Employee ID</t>
+  </si>
+  <si>
+    <t>Bar Council ID Card</t>
+  </si>
+  <si>
+    <t>Leaving certificate/Admit Card/10th Class certificate</t>
+  </si>
+  <si>
+    <t>Municipal Birth Certificate</t>
+  </si>
+  <si>
+    <t>High School</t>
+  </si>
+  <si>
+    <t>Graduate</t>
+  </si>
+  <si>
+    <t>Post Graduate</t>
+  </si>
+  <si>
+    <t>Professional</t>
+  </si>
+  <si>
+    <t>Diploma</t>
+  </si>
+  <si>
+    <t>Illiterate</t>
+  </si>
+  <si>
+    <t>Primary School</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>Divorced</t>
+  </si>
+  <si>
+    <t>Widow</t>
+  </si>
+  <si>
+    <t>Widower</t>
+  </si>
+  <si>
+    <t>educationInsurersDetails</t>
+  </si>
+  <si>
+    <t>maritalStatus</t>
+  </si>
+  <si>
+    <t>Govt</t>
+  </si>
+  <si>
+    <t>Pvt Ltd</t>
+  </si>
+  <si>
+    <t>Public Ltd</t>
+  </si>
+  <si>
+    <t>Partner/Prop</t>
+  </si>
+  <si>
+    <t>Trust</t>
+  </si>
+  <si>
+    <t>Society</t>
+  </si>
+  <si>
+    <t>Non-Governmental Organization (NGO)</t>
+  </si>
+  <si>
+    <t>Non-Profit organization (NPO)</t>
+  </si>
+  <si>
+    <t>Private Voluntary Organization (PVO)</t>
+  </si>
+  <si>
+    <t>Not Applicable</t>
+  </si>
+  <si>
+    <t>organizationType</t>
+  </si>
+  <si>
+    <t>Defence</t>
+  </si>
+  <si>
+    <t>Diving</t>
+  </si>
+  <si>
+    <t>Oil &amp; Natural Gas</t>
+  </si>
+  <si>
+    <t>Merchant Marine</t>
+  </si>
+  <si>
+    <t>Mining</t>
+  </si>
+  <si>
+    <t>Aviation</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Self Employed</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Self Employed From Home</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Agriculture</t>
+  </si>
+  <si>
+    <t>Housewife</t>
+  </si>
+  <si>
+    <t>Retired</t>
+  </si>
+  <si>
+    <t>250000000</t>
+  </si>
+  <si>
+    <t>350000000</t>
+  </si>
+  <si>
+    <t>1000000</t>
+  </si>
+  <si>
+    <t>2000000</t>
+  </si>
+  <si>
+    <t>3000000</t>
+  </si>
+  <si>
+    <t>300000</t>
+  </si>
+  <si>
+    <t>400000</t>
+  </si>
+  <si>
+    <t>360000000</t>
+  </si>
+  <si>
+    <t>370000000</t>
+  </si>
+  <si>
+    <t>700</t>
+  </si>
+  <si>
+    <t>premiumCommitmentWLS</t>
+  </si>
+  <si>
+    <t>Min Premium is Rs.50000</t>
+  </si>
+  <si>
+    <t>Min Annual Income is Rs. 64800</t>
+  </si>
+  <si>
+    <t>errorMsgValidationForMIAP</t>
+  </si>
+  <si>
+    <t>errorMsgValidationForWLS</t>
+  </si>
+  <si>
+    <t>errorMsgValidationForSTP</t>
+  </si>
+  <si>
+    <t>100000</t>
+  </si>
+  <si>
+    <t>Minimum Premium is 8500</t>
+  </si>
+  <si>
+    <t>Minimum SA for 10</t>
+  </si>
+  <si>
+    <t>15 and 20 years PPT is 50000</t>
+  </si>
+  <si>
+    <t>Minimum Premium is 8500</t>
+  </si>
+  <si>
+    <t>errorMsgValidationWLSPremiumCommitment</t>
+  </si>
+  <si>
+    <t>errorMsgValidationWLSPremiumCommitment=700</t>
+  </si>
+  <si>
+    <t>errorMsgValidationPremiumCommitmentWLS=700</t>
+  </si>
+  <si>
+    <t>Minimum SA for 10, 15 and 20 years PPT is 50000</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Minimum ,Premium ,is 8500</t>
+  </si>
+  <si>
+    <t>errorMsgValidationForSAP=PremiumCommitmmnet=400000</t>
+  </si>
+  <si>
+    <t>Maximum SA for Waiver of Premium Plus Rider is Rs. 350000.</t>
+  </si>
+  <si>
+    <t>Minimum Annualised Premium should be 10000/-. Enter higher Premium amount</t>
+  </si>
+  <si>
+    <t>errorMsgValidationForSAP=PremiumCommitmmnet=700</t>
+  </si>
+  <si>
+    <t>errorMsgValidationForSAP=PremiumCommitmmnet=370000000</t>
+  </si>
+  <si>
+    <t>Minimum Sum Assured is Rs. 2500000</t>
+  </si>
+  <si>
+    <t>Minimum premium for Annual mode is Rs. 5000</t>
+  </si>
+  <si>
+    <t>Rider not applicable as sum at risk is lower than permitted</t>
+  </si>
+  <si>
+    <t>Fund1</t>
+  </si>
+  <si>
+    <t>Fund2</t>
+  </si>
+  <si>
+    <t>Fund3</t>
+  </si>
+  <si>
+    <t>Fund4</t>
+  </si>
+  <si>
+    <t>Fund5</t>
+  </si>
+  <si>
+    <t>Fund6</t>
+  </si>
+  <si>
+    <t>premiunCommitmentFTS</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>AND@B0001899q</t>
+  </si>
+  <si>
+    <t>78101@1005w</t>
+  </si>
+  <si>
+    <t>Beltola Btl</t>
+  </si>
+  <si>
+    <t>bankBranchPrepopulatedDataValidation</t>
+  </si>
+  <si>
+    <t>ANDHRA BANK</t>
+  </si>
+  <si>
+    <t>bankNamePrepopulatedDataValidation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adolph.@ Blaine Charles David Earl Frederick Gerald Hubert Irvim John Kenneth Loyd Martin Nero Oliver Paul Quincy Randolph Sherman Thomas Uncas Victor Willian </t>
+  </si>
+  <si>
+    <t>2313424E32432342222344</t>
+  </si>
+  <si>
+    <t>dropDownOftypeOfAccountBankDetails</t>
+  </si>
+  <si>
+    <t>Savings Account</t>
+  </si>
+  <si>
+    <t>Current Account</t>
+  </si>
+  <si>
+    <t>Cash Credit</t>
+  </si>
+  <si>
+    <t>NRE</t>
+  </si>
+  <si>
+    <t>NRO</t>
+  </si>
+  <si>
+    <t>3313424E72432342222344</t>
+  </si>
+  <si>
+    <t>4313424E32432342222344</t>
+  </si>
+  <si>
+    <t>5313424E32432642222344</t>
+  </si>
+  <si>
+    <t>6313424E32432342222344</t>
+  </si>
+  <si>
+    <t>7313424E32432342222344</t>
+  </si>
+  <si>
+    <t>8313424E32432342222344</t>
+  </si>
+  <si>
+    <t>9313424E32432342222344</t>
+  </si>
+  <si>
+    <t>SBIN0001537</t>
+  </si>
+  <si>
+    <t>ICIC0006561</t>
+  </si>
+  <si>
+    <t>UTIB0000373</t>
+  </si>
+  <si>
+    <t>HDFC0001015</t>
+  </si>
+  <si>
+    <t>SBI</t>
+  </si>
+  <si>
+    <t>110002022</t>
+  </si>
+  <si>
+    <t>FathersName</t>
+  </si>
+  <si>
+    <t>Adolph@. Blaine Charles. David Earl Frederick Gerald Hubert Irvim John Kenneth Loyd Martin Nero Oliver Paul Quincy Randolph Sherman Thomas Uncas Victor Willian Xerxes Yancy Zeus Wolfeschlegelsteinhausenbergerdorffvoralternwarengewissenh</t>
+  </si>
+  <si>
+    <t>MothersName</t>
+  </si>
+  <si>
+    <t>DropDownListMaritalStatusPersonalDetails</t>
+  </si>
+  <si>
+    <t>DropDownListEducationPersonalDetails</t>
+  </si>
+  <si>
+    <t>Merchant Marine/Navy</t>
+  </si>
+  <si>
+    <t>Aviation/AirForce"</t>
+  </si>
+  <si>
+    <t>DropDownIndustryType</t>
+  </si>
+  <si>
+    <t>DropDownIndustryType-Merchant Marine/Navy</t>
+  </si>
+  <si>
+    <t>Passenger/Ferry</t>
+  </si>
+  <si>
+    <t>Cargo Vessel</t>
+  </si>
+  <si>
+    <t>Oil Tanker</t>
+  </si>
+  <si>
+    <t>Vessel carrying Chemicals/Explosives</t>
+  </si>
+  <si>
+    <t>Submarines</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Non-Profit organization (NPO)</t>
+  </si>
+  <si>
+    <t>Salaried</t>
+  </si>
+  <si>
+    <t>Agriculture</t>
+  </si>
+  <si>
+    <t>DropDownOrganizationType</t>
+  </si>
+  <si>
+    <t>DropDownOccupation</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>Spouse</t>
+  </si>
+  <si>
+    <t>Brother</t>
+  </si>
+  <si>
+    <t>Sister</t>
+  </si>
+  <si>
+    <t>Grand Parent</t>
+  </si>
+  <si>
+    <t>DropDownProposerRelationshipWithNominee</t>
+  </si>
+  <si>
+    <t>Adolph. Blaine#1@ Charles David Earl Frederick Gerald Hubert Irvim John Kenneth</t>
+  </si>
+  <si>
+    <t>Adolph. Blaine@ Charles David Earl Frederick Gerald Hubert Irvim John Kenneth</t>
+  </si>
+  <si>
+    <t>WeightPersonalDetails</t>
+  </si>
+  <si>
+    <t>InsurerOtherDetailsAnnualIncome</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -201,16 +696,35 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -218,12 +732,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -245,6 +774,41 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -543,7 +1107,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -594,12 +1158,292 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" customWidth="1"/>
+    <col min="4" max="4" width="39.7109375" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" customWidth="1"/>
+    <col min="7" max="7" width="31.42578125" customWidth="1"/>
+    <col min="8" max="8" width="25.85546875" customWidth="1"/>
+    <col min="9" max="9" width="38.5703125" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="45">
+      <c r="A1" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="195">
+      <c r="A2" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="I2" t="s">
+        <v>200</v>
+      </c>
+      <c r="J2">
+        <v>50</v>
+      </c>
+      <c r="K2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="I3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="I5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="I6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="I7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" s="25"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -609,10 +1453,15 @@
     <col min="3" max="3" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" customWidth="1"/>
     <col min="5" max="5" width="31.42578125" customWidth="1"/>
-    <col min="6" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" customWidth="1"/>
+    <col min="7" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="45" customWidth="1"/>
+    <col min="10" max="10" width="24.140625" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" style="13" customWidth="1"/>
+    <col min="12" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:11" ht="45">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -628,16 +1477,34 @@
       <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -645,15 +1512,65 @@
       <c r="E2">
         <v>98760987123</v>
       </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2">
+        <v>999</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="J2" s="10">
+        <v>33277</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="H9" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="C2" r:id="rId2"/>
     <hyperlink ref="B2" r:id="rId3"/>
+    <hyperlink ref="I2" r:id="rId4" display="QQQQQQQQQQQQQQQQQQQQ1@QQQQQQQQQQQQQQQQQQQQQQQQQQQQQQ"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -663,15 +1580,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D1:H2"/>
+  <dimension ref="D1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="4:8" ht="75">
+    <row r="1" spans="4:9" ht="30">
       <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
@@ -687,13 +1608,14 @@
       <c r="H1" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="4:8">
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="4:9">
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -720,10 +1642,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H10" activeCellId="1" sqref="H2 H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -734,11 +1656,19 @@
     <col min="4" max="4" width="39.5703125" customWidth="1"/>
     <col min="5" max="5" width="19.85546875" customWidth="1"/>
     <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" customWidth="1"/>
     <col min="10" max="10" width="13.85546875" customWidth="1"/>
     <col min="11" max="11" width="30.7109375" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" customWidth="1"/>
+    <col min="16" max="16" width="27.7109375" customWidth="1"/>
+    <col min="18" max="18" width="24" customWidth="1"/>
+    <col min="20" max="20" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -772,115 +1702,1095 @@
       <c r="K1" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="60" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>44</v>
+        <v>206</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="C2" s="5">
         <v>35291</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" s="8" t="s">
+      <c r="L2" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q2" s="11">
+        <v>10</v>
+      </c>
+      <c r="R2" t="s">
+        <v>69</v>
+      </c>
+      <c r="S2" t="s">
+        <v>76</v>
+      </c>
+      <c r="T2" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="M3" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="N3" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="O3" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="P3" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q3" s="11"/>
+      <c r="R3" t="s">
+        <v>70</v>
+      </c>
+      <c r="S3" t="s">
+        <v>77</v>
+      </c>
+      <c r="T3" s="20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="L4" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="P4" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q4" s="11">
+        <v>10</v>
+      </c>
+      <c r="R4" t="s">
+        <v>71</v>
+      </c>
+      <c r="S4" t="s">
+        <v>78</v>
+      </c>
+      <c r="T4" s="20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="L5" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="N5" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="O5" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="P5" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q5" s="11">
+        <v>10</v>
+      </c>
+      <c r="R5" t="s">
+        <v>72</v>
+      </c>
+      <c r="S5" t="s">
+        <v>79</v>
+      </c>
+      <c r="T5" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="L6" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="M6" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="N6" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="O6" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="P6" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q6" s="11">
+        <v>10</v>
+      </c>
+      <c r="R6" t="s">
+        <v>73</v>
+      </c>
+      <c r="S6" t="s">
+        <v>80</v>
+      </c>
+      <c r="T6" s="20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="L7" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="M7" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="N7" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="O7" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="P7" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q7" s="11">
+        <v>10</v>
+      </c>
+      <c r="R7" t="s">
+        <v>74</v>
+      </c>
+      <c r="T7" s="20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="L8" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="N8" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="O8" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="P8" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q8" s="11">
         <v>50</v>
       </c>
-      <c r="K2" s="8" t="s">
-        <v>51</v>
+      <c r="R8" t="s">
+        <v>75</v>
+      </c>
+      <c r="T8" s="20" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="TestFirstName1@wwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwwww"/>
-    <hyperlink ref="J2" r:id="rId2"/>
-    <hyperlink ref="K2" r:id="rId3"/>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="K2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="1" max="1" width="94.140625" customWidth="1"/>
+    <col min="2" max="2" width="88.42578125" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
     <col min="5" max="5" width="25.28515625" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" customWidth="1"/>
+    <col min="6" max="6" width="56" customWidth="1"/>
+    <col min="7" max="7" width="65" customWidth="1"/>
+    <col min="8" max="8" width="45" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" customWidth="1"/>
+    <col min="11" max="11" width="36.7109375" customWidth="1"/>
+    <col min="12" max="12" width="39.140625" customWidth="1"/>
+    <col min="13" max="13" width="41.5703125" customWidth="1"/>
+    <col min="14" max="14" width="39.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>26</v>
       </c>
       <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" t="s">
+        <v>157</v>
+      </c>
+      <c r="L1" t="s">
+        <v>159</v>
+      </c>
+      <c r="M1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="62.25" customHeight="1">
-      <c r="A2" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="B2" s="6" t="s">
-        <v>27</v>
+        <v>94</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K2" t="s">
+        <v>156</v>
+      </c>
+      <c r="L2" t="s">
+        <v>158</v>
+      </c>
+      <c r="M2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="E3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="H3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="H4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" t="s">
+        <v>78</v>
+      </c>
+      <c r="M4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="B5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="H5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I5" t="s">
+        <v>72</v>
+      </c>
+      <c r="J5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="H6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" t="s">
+        <v>80</v>
+      </c>
+      <c r="M6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="B7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="H7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="B8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="H8" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="C9" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="H9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="C10" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="H10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="G2" r:id="rId3"/>
+    <hyperlink ref="G3:G10" r:id="rId4" display="Adolph.@ Blaine Charles David Earl Frederick Gerald Hubert Irvim John Kenneth Loyd Martin Nero Oliver Paul Quincy Randolph Sherman Thomas Uncas Victor Willian "/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26:C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="17"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>94</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>39</v>
-      </c>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="C11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="65.7109375" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" customWidth="1"/>
+    <col min="3" max="3" width="39.140625" customWidth="1"/>
+    <col min="4" max="4" width="45" customWidth="1"/>
+    <col min="5" max="5" width="51.140625" customWidth="1"/>
+    <col min="6" max="8" width="55.42578125" customWidth="1"/>
+    <col min="9" max="9" width="61.85546875" customWidth="1"/>
+    <col min="10" max="10" width="52.85546875" customWidth="1"/>
+    <col min="11" max="11" width="63.28515625" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" customWidth="1"/>
+    <col min="13" max="13" width="25.28515625" customWidth="1"/>
+    <col min="14" max="14" width="27.5703125" customWidth="1"/>
+    <col min="15" max="15" width="33.5703125" customWidth="1"/>
+    <col min="16" max="16" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:F2"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M16" activeCellId="1" sqref="P2 M16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="69.7109375" customWidth="1"/>
+    <col min="2" max="2" width="55" customWidth="1"/>
+    <col min="3" max="3" width="63.85546875" customWidth="1"/>
+    <col min="4" max="4" width="65.85546875" customWidth="1"/>
+    <col min="5" max="5" width="83.85546875" customWidth="1"/>
+    <col min="6" max="6" width="78" customWidth="1"/>
+    <col min="7" max="8" width="29.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6">
+      <c r="B1" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6">
+      <c r="B2" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" activeCellId="1" sqref="G2 G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" customWidth="1"/>
+    <col min="8" max="8" width="30.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="20"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="11"/>
+      <c r="H8" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updating latest requirement change
</commit_message>
<xml_diff>
--- a/src/test/resources/MasterData.xlsx
+++ b/src/test/resources/MasterData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="743" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="743" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="226">
   <si>
     <t>username</t>
   </si>
@@ -190,12 +190,6 @@
   </si>
   <si>
     <t>Fund</t>
-  </si>
-  <si>
-    <t>erroMessage</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>500000</t>
@@ -671,6 +665,54 @@
   <si>
     <t xml:space="preserve">We
 </t>
+  </si>
+  <si>
+    <t>2344</t>
+  </si>
+  <si>
+    <t>233333</t>
+  </si>
+  <si>
+    <t>2889</t>
+  </si>
+  <si>
+    <t>23339999</t>
+  </si>
+  <si>
+    <t>2333000</t>
+  </si>
+  <si>
+    <t>233339111111111111111111</t>
+  </si>
+  <si>
+    <t>CPYPP4044C@</t>
+  </si>
+  <si>
+    <t>22222</t>
+  </si>
+  <si>
+    <t>2222</t>
+  </si>
+  <si>
+    <t>3333</t>
+  </si>
+  <si>
+    <t>444</t>
+  </si>
+  <si>
+    <t>555</t>
+  </si>
+  <si>
+    <t>navneetgmail.com</t>
+  </si>
+  <si>
+    <t>navneet@gmailcom</t>
+  </si>
+  <si>
+    <t>navneet@gmail.</t>
+  </si>
+  <si>
+    <t>navneet@com</t>
   </si>
 </sst>
 </file>
@@ -752,7 +794,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -809,6 +851,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1182,66 +1225,66 @@
   <sheetData>
     <row r="1" spans="1:11" ht="45">
       <c r="A1" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="C1" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" s="24" t="s">
         <v>183</v>
       </c>
-      <c r="C1" s="24" t="s">
-        <v>184</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>185</v>
-      </c>
       <c r="E1" s="24" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I1" s="24" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J1" s="24" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="K1" s="24" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="195">
       <c r="A2" s="24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J2">
         <v>50</v>
@@ -1254,100 +1297,100 @@
       <c r="A3" s="25"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="25"/>
       <c r="B4" s="25"/>
       <c r="C4" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="25"/>
       <c r="B5" s="25"/>
       <c r="C5" s="25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H5" s="25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="25"/>
       <c r="B6" s="25"/>
       <c r="C6" s="25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1355,20 +1398,20 @@
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
       <c r="D7" s="25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1376,17 +1419,17 @@
       <c r="B8" s="25"/>
       <c r="C8" s="25"/>
       <c r="D8" s="25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F8" s="25"/>
       <c r="G8" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1397,10 +1440,10 @@
       <c r="E9" s="25"/>
       <c r="F9" s="25"/>
       <c r="G9" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1411,10 +1454,10 @@
       <c r="E10" s="25"/>
       <c r="F10" s="25"/>
       <c r="G10" s="25" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1425,7 +1468,7 @@
       <c r="E11" s="25"/>
       <c r="F11" s="25"/>
       <c r="G11" s="25" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H11" s="25"/>
     </row>
@@ -1442,14 +1485,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" customWidth="1"/>
     <col min="5" max="5" width="31.42578125" customWidth="1"/>
@@ -1492,12 +1535,10 @@
       <c r="J1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="12" t="s">
-        <v>54</v>
-      </c>
+      <c r="K1" s="12"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" t="s">
+      <c r="A2" s="14" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -1518,59 +1559,118 @@
       <c r="G2" t="s">
         <v>43</v>
       </c>
-      <c r="H2">
-        <v>999</v>
+      <c r="H2" t="s">
+        <v>43</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="J2" s="10">
         <v>33277</v>
       </c>
-      <c r="K2" s="13" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="B3" s="8"/>
+      <c r="A3" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>217</v>
+      </c>
       <c r="C3" s="8"/>
+      <c r="D3" t="s">
+        <v>222</v>
+      </c>
       <c r="I3" s="6"/>
       <c r="J3" s="10"/>
       <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="B4" s="8"/>
+      <c r="A4" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>218</v>
+      </c>
       <c r="C4" s="8"/>
+      <c r="D4" t="s">
+        <v>223</v>
+      </c>
       <c r="I4" s="6"/>
       <c r="J4" s="10"/>
       <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="B5" s="8"/>
+      <c r="A5" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>219</v>
+      </c>
       <c r="C5" s="8"/>
+      <c r="D5" t="s">
+        <v>224</v>
+      </c>
       <c r="I5" s="6"/>
       <c r="J5" s="10"/>
       <c r="K5" s="6"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="B6" s="8"/>
+      <c r="A6" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>220</v>
+      </c>
       <c r="C6" s="8"/>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
       <c r="I6" s="6"/>
       <c r="J6" s="10"/>
       <c r="K6" s="6"/>
     </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="D7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="9" spans="1:11">
+      <c r="A9" s="14"/>
       <c r="H9" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="B2" r:id="rId3"/>
-    <hyperlink ref="I2" r:id="rId4" display="QQQQQQQQQQQQQQQQQQQQ1@QQQQQQQQQQQQQQQQQQQQQQQQQQQQQQ"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="I2" r:id="rId3" display="QQQQQQQQQQQQQQQQQQQQ1@QQQQQQQQQQQQQQQQQQQQQQQQQQQQQQ"/>
+    <hyperlink ref="B8" r:id="rId4"/>
+    <hyperlink ref="D8" r:id="rId5"/>
+    <hyperlink ref="D5" r:id="rId6"/>
+    <hyperlink ref="D4" r:id="rId7"/>
+    <hyperlink ref="D3" r:id="rId8" display="navneet@gmail.com"/>
+    <hyperlink ref="D6" r:id="rId9"/>
+    <hyperlink ref="D7" r:id="rId10"/>
+    <hyperlink ref="D2" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1644,7 +1744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="H10" activeCellId="1" sqref="H2 H10"/>
     </sheetView>
   </sheetViews>
@@ -1715,16 +1815,16 @@
         <v>51</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>53</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="T1" s="4" t="s">
         <v>52</v>
@@ -1732,31 +1832,31 @@
     </row>
     <row r="2" spans="1:20" ht="60" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C2" s="5">
         <v>35291</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>39</v>
@@ -1765,31 +1865,31 @@
         <v>47</v>
       </c>
       <c r="L2" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="N2" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="O2" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="N2" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="O2" s="21" t="s">
-        <v>111</v>
-      </c>
       <c r="P2" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="Q2" s="11">
         <v>10</v>
       </c>
       <c r="R2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="S2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="T2" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -1805,168 +1905,168 @@
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M3" s="20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="N3" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="O3" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P3" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="Q3" s="11"/>
       <c r="R3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="S3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="T3" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="L4" s="20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N4" s="20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O4" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="P4" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Q4" s="11">
         <v>10</v>
       </c>
       <c r="R4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="S4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="T4" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="L5" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M5" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="N5" s="21" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="O5" s="21" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P5" s="21" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="Q5" s="11">
         <v>10</v>
       </c>
       <c r="R5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="S5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T5" s="21" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="L6" s="20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N6" s="20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O6" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="P6" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Q6" s="11">
         <v>10</v>
       </c>
       <c r="R6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="S6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="T6" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="L7" s="20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M7" s="20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N7" s="20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O7" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="P7" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Q7" s="11">
         <v>10</v>
       </c>
       <c r="R7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="T7" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="L8" s="20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M8" s="20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N8" s="20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O8" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="P8" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Q8" s="11">
         <v>50</v>
       </c>
       <c r="R8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="T8" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2028,16 +2128,16 @@
         <v>33</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K1" t="s">
+        <v>155</v>
+      </c>
+      <c r="L1" t="s">
         <v>157</v>
       </c>
-      <c r="L1" t="s">
-        <v>159</v>
-      </c>
       <c r="M1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
@@ -2045,239 +2145,239 @@
         <v>28</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>46</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" t="s">
+        <v>154</v>
+      </c>
+      <c r="L2" t="s">
+        <v>156</v>
+      </c>
+      <c r="M2" t="s">
         <v>161</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="I2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K2" t="s">
-        <v>156</v>
-      </c>
-      <c r="L2" t="s">
-        <v>158</v>
-      </c>
-      <c r="M2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="B3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="M3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="B4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="B5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="B6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="B7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="B8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="C9" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="C10" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2310,122 +2410,122 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D1" s="17"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="C9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="C10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="C11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2461,28 +2561,28 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="22" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D1" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>130</v>
-      </c>
       <c r="G1" s="22" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I1" s="22"/>
       <c r="J1" s="22"/>
@@ -2495,28 +2595,28 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D2" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>127</v>
-      </c>
       <c r="G2" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
@@ -2524,17 +2624,17 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
@@ -2545,15 +2645,15 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
@@ -2588,36 +2688,36 @@
   <sheetData>
     <row r="1" spans="2:6">
       <c r="B1" s="22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2642,140 +2742,140 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>146</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="C2" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="F2" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>153</v>
-      </c>
       <c r="G2" s="21" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:8">

</xml_diff>

<commit_message>
Latest updated of enabled code
</commit_message>
<xml_diff>
--- a/src/test/resources/MasterData.xlsx
+++ b/src/test/resources/MasterData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="743" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="743" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="337">
   <si>
     <t>username</t>
   </si>
@@ -133,12 +133,6 @@
   </si>
   <si>
     <t>CEZPK29019#</t>
-  </si>
-  <si>
-    <t>669228772880*A</t>
-  </si>
-  <si>
-    <t>9873901989A@</t>
   </si>
   <si>
     <t>CPYPP4048C@</t>
@@ -429,9 +423,6 @@
     <t/>
   </si>
   <si>
-    <t>Minimum ,Premium ,is 8500</t>
-  </si>
-  <si>
     <t>errorMsgValidationForSAP=PremiumCommitmmnet=400000</t>
   </si>
   <si>
@@ -667,24 +658,6 @@
 </t>
   </si>
   <si>
-    <t>2344</t>
-  </si>
-  <si>
-    <t>233333</t>
-  </si>
-  <si>
-    <t>2889</t>
-  </si>
-  <si>
-    <t>23339999</t>
-  </si>
-  <si>
-    <t>2333000</t>
-  </si>
-  <si>
-    <t>233339111111111111111111</t>
-  </si>
-  <si>
     <t>CPYPP4044C@</t>
   </si>
   <si>
@@ -703,9 +676,6 @@
     <t>555</t>
   </si>
   <si>
-    <t>navneetgmail.com</t>
-  </si>
-  <si>
     <t>navneet@gmailcom</t>
   </si>
   <si>
@@ -713,6 +683,369 @@
   </si>
   <si>
     <t>navneet@com</t>
+  </si>
+  <si>
+    <t>navneet@monocept.com</t>
+  </si>
+  <si>
+    <t>suniti@monocept.com</t>
+  </si>
+  <si>
+    <t>9873970332</t>
+  </si>
+  <si>
+    <t>9717277996</t>
+  </si>
+  <si>
+    <t>9873970332A@</t>
+  </si>
+  <si>
+    <t>98739A@</t>
+  </si>
+  <si>
+    <t>9870332A@</t>
+  </si>
+  <si>
+    <t>987397032A@</t>
+  </si>
+  <si>
+    <t>987332A@</t>
+  </si>
+  <si>
+    <t>FirstNamePosvTestDataSAP</t>
+  </si>
+  <si>
+    <t>FirstNamePosvTestDataMIAP</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>9888819288@</t>
+  </si>
+  <si>
+    <t>gaur.manojk@gmail.com</t>
+  </si>
+  <si>
+    <t>8374848595@</t>
+  </si>
+  <si>
+    <t>123456789123</t>
+  </si>
+  <si>
+    <t>1234567891</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>1234567</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>123456789121</t>
+  </si>
+  <si>
+    <t>rimpi.poddar@gmail.com</t>
+  </si>
+  <si>
+    <t>Lindsey Craft</t>
+  </si>
+  <si>
+    <t>Erica Larsen</t>
+  </si>
+  <si>
+    <t>Ryan Levine</t>
+  </si>
+  <si>
+    <t>Erika Smith</t>
+  </si>
+  <si>
+    <t>Brooklyn Sloan</t>
+  </si>
+  <si>
+    <t>Karen Mayer</t>
+  </si>
+  <si>
+    <t>Eddie O'neill</t>
+  </si>
+  <si>
+    <t>Nancy Stevens</t>
+  </si>
+  <si>
+    <t>Chasity Conway</t>
+  </si>
+  <si>
+    <t>Aaron McCray</t>
+  </si>
+  <si>
+    <t>Kendra Allen</t>
+  </si>
+  <si>
+    <t>Jenna Burns</t>
+  </si>
+  <si>
+    <t>Jane Mayo</t>
+  </si>
+  <si>
+    <t>George Suarez</t>
+  </si>
+  <si>
+    <t>Janet Abbott</t>
+  </si>
+  <si>
+    <t>Steven Marshall</t>
+  </si>
+  <si>
+    <t>Shane Heath</t>
+  </si>
+  <si>
+    <t>Unborn Vega</t>
+  </si>
+  <si>
+    <t>Kaitlyn Wilder</t>
+  </si>
+  <si>
+    <t>Donald Morgan</t>
+  </si>
+  <si>
+    <t>Alisha Dunn</t>
+  </si>
+  <si>
+    <t>Marty Franco</t>
+  </si>
+  <si>
+    <t>Sam Jackson</t>
+  </si>
+  <si>
+    <t>Jeffrey Suarez</t>
+  </si>
+  <si>
+    <t>Thomas Dotson</t>
+  </si>
+  <si>
+    <t>Mickey Cruz</t>
+  </si>
+  <si>
+    <t>Chuck Castillo</t>
+  </si>
+  <si>
+    <t>Sierra Schneider</t>
+  </si>
+  <si>
+    <t>Michael Gross</t>
+  </si>
+  <si>
+    <t>Richard Wheeler</t>
+  </si>
+  <si>
+    <t>Margaret Kane</t>
+  </si>
+  <si>
+    <t>Hope Compton</t>
+  </si>
+  <si>
+    <t>Helen Richmond</t>
+  </si>
+  <si>
+    <t>Myron Hayes</t>
+  </si>
+  <si>
+    <t>Laura Richardson</t>
+  </si>
+  <si>
+    <t>Patrick Walker</t>
+  </si>
+  <si>
+    <t>Kaylee Austin</t>
+  </si>
+  <si>
+    <t>Timmy Green</t>
+  </si>
+  <si>
+    <t>Terry Roberson</t>
+  </si>
+  <si>
+    <t>Donnie Nunez</t>
+  </si>
+  <si>
+    <t>Rick O'neal</t>
+  </si>
+  <si>
+    <t>Dave Chang</t>
+  </si>
+  <si>
+    <t>Carrie McDowell</t>
+  </si>
+  <si>
+    <t>Brenda Flynn</t>
+  </si>
+  <si>
+    <t>Kaitlyn Kerr</t>
+  </si>
+  <si>
+    <t>Sandra Love</t>
+  </si>
+  <si>
+    <t>Donna Navarro</t>
+  </si>
+  <si>
+    <t>Vernon Lloyd</t>
+  </si>
+  <si>
+    <t>Greg Hahn</t>
+  </si>
+  <si>
+    <t>Brad Mays</t>
+  </si>
+  <si>
+    <t>Greg Melton</t>
+  </si>
+  <si>
+    <t>Ernest Daniel</t>
+  </si>
+  <si>
+    <t>Whitney Davenport</t>
+  </si>
+  <si>
+    <t>Wendy Carson</t>
+  </si>
+  <si>
+    <t>Juanita Short</t>
+  </si>
+  <si>
+    <t>Louis Guthrie</t>
+  </si>
+  <si>
+    <t>Barb Maddox</t>
+  </si>
+  <si>
+    <t>Chelsea Hurst</t>
+  </si>
+  <si>
+    <t>Katrina Sherman</t>
+  </si>
+  <si>
+    <t>Kelly Morse</t>
+  </si>
+  <si>
+    <t>Nancy Merritt</t>
+  </si>
+  <si>
+    <t>Marion Cash</t>
+  </si>
+  <si>
+    <t>Brent Richards</t>
+  </si>
+  <si>
+    <t>Cassandra Lindsay</t>
+  </si>
+  <si>
+    <t>Ray Bates</t>
+  </si>
+  <si>
+    <t>Christina McMillan</t>
+  </si>
+  <si>
+    <t>Candy Walton</t>
+  </si>
+  <si>
+    <t>Joanne Copeland</t>
+  </si>
+  <si>
+    <t>Skyler Murray</t>
+  </si>
+  <si>
+    <t>Charlotte Nolan</t>
+  </si>
+  <si>
+    <t>Ruth Kinney</t>
+  </si>
+  <si>
+    <t>Craig Avila</t>
+  </si>
+  <si>
+    <t>Billy Middleton</t>
+  </si>
+  <si>
+    <t>Dixie Avery</t>
+  </si>
+  <si>
+    <t>Erika Andrews</t>
+  </si>
+  <si>
+    <t>Brett Camacho</t>
+  </si>
+  <si>
+    <t>Frank Leonard</t>
+  </si>
+  <si>
+    <t>Justin Henry</t>
+  </si>
+  <si>
+    <t>Juanita Clements</t>
+  </si>
+  <si>
+    <t>Rob Ruiz</t>
+  </si>
+  <si>
+    <t>Jean Pugh</t>
+  </si>
+  <si>
+    <t>Gina Lyons</t>
+  </si>
+  <si>
+    <t>Lewis Holman</t>
+  </si>
+  <si>
+    <t>Justin Watson</t>
+  </si>
+  <si>
+    <t>Ronda Hopper</t>
+  </si>
+  <si>
+    <t>Lance Cooley</t>
+  </si>
+  <si>
+    <t>Tamara Perez</t>
+  </si>
+  <si>
+    <t>Daniel Stanton</t>
+  </si>
+  <si>
+    <t>Ann Shaffer</t>
+  </si>
+  <si>
+    <t>Curtis Hutchinson</t>
+  </si>
+  <si>
+    <t>Rachel Melton</t>
+  </si>
+  <si>
+    <t>Brittany Sweeney</t>
+  </si>
+  <si>
+    <t>Nicole Ballard</t>
+  </si>
+  <si>
+    <t>Kaylee Wall</t>
+  </si>
+  <si>
+    <t>Brad Gaines</t>
+  </si>
+  <si>
+    <t>Matt Kerr</t>
+  </si>
+  <si>
+    <t>Kelly Fuller</t>
+  </si>
+  <si>
+    <t>Christina Rosa</t>
   </si>
 </sst>
 </file>
@@ -722,7 +1055,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -747,6 +1080,19 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -794,7 +1140,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -821,7 +1167,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -852,6 +1197,8 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1205,9 +1552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1224,67 +1569,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="45">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1" s="23" t="s">
         <v>183</v>
       </c>
-      <c r="E1" s="24" t="s">
-        <v>186</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>187</v>
-      </c>
-      <c r="G1" s="24" t="s">
-        <v>196</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="I1" s="24" t="s">
+      <c r="F1" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="J1" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="J1" s="24" t="s">
-        <v>206</v>
-      </c>
-      <c r="K1" s="24" t="s">
-        <v>207</v>
+      <c r="K1" s="23" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="195">
-      <c r="A2" s="24" t="s">
-        <v>180</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>180</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>194</v>
+      <c r="A2" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>191</v>
       </c>
       <c r="I2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="J2">
         <v>50</v>
@@ -1294,183 +1639,183 @@
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25" t="s">
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="I3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D5" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="F3" s="25" t="s">
+      <c r="E5" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="I5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="G3" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="H3" s="25" t="s">
+      <c r="G6" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I6" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="F4" s="25" t="s">
+    <row r="7" spans="1:11">
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="I7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24" t="s">
         <v>190</v>
       </c>
-      <c r="G4" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="H4" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="I4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="F5" s="25" t="s">
-        <v>191</v>
-      </c>
-      <c r="G5" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="H5" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="I5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="E6" s="25" t="s">
+      <c r="H9" s="24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="F6" s="25" t="s">
-        <v>192</v>
-      </c>
-      <c r="G6" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="H6" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="I6" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="25"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="H7" s="25" t="s">
-        <v>195</v>
-      </c>
-      <c r="I7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="H8" s="25" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25" t="s">
-        <v>193</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="H10" s="25" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="H11" s="25"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" s="24"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1483,24 +1828,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" customWidth="1"/>
     <col min="5" max="5" width="31.42578125" customWidth="1"/>
     <col min="6" max="6" width="33.140625" customWidth="1"/>
     <col min="7" max="8" width="8.7109375" customWidth="1"/>
     <col min="9" max="9" width="45" customWidth="1"/>
     <col min="10" max="10" width="24.140625" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" style="13" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" style="12" customWidth="1"/>
     <col min="12" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1511,166 +1854,229 @@
       <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="I1" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="12"/>
+      <c r="K1" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>37</v>
-      </c>
       <c r="C2" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
+        <v>230</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>229</v>
       </c>
       <c r="E2">
         <v>98760987123</v>
       </c>
       <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
         <v>41</v>
       </c>
-      <c r="G2" t="s">
-        <v>43</v>
-      </c>
       <c r="H2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="J2" s="10">
         <v>33277</v>
       </c>
+      <c r="K2" s="13" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>217</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" t="s">
-        <v>222</v>
+      <c r="A3" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="10"/>
-      <c r="K3" s="6"/>
+      <c r="K3" s="13" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>218</v>
-      </c>
-      <c r="C4" s="8"/>
+      <c r="A4" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>222</v>
+      </c>
       <c r="D4" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="10"/>
-      <c r="K4" s="6"/>
+      <c r="K4" s="13" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>219</v>
-      </c>
-      <c r="C5" s="8"/>
+      <c r="A5" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>223</v>
+      </c>
       <c r="D5" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="10"/>
-      <c r="K5" s="6"/>
+      <c r="K5" s="13" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>220</v>
-      </c>
-      <c r="C6" s="8"/>
+      <c r="A6" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>224</v>
+      </c>
       <c r="D6" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="10"/>
-      <c r="K6" s="6"/>
+      <c r="K6" s="13" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="14" t="s">
-        <v>214</v>
-      </c>
-      <c r="B7" s="26" t="s">
+      <c r="A7" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>221</v>
       </c>
       <c r="D7" t="s">
-        <v>225</v>
+        <v>215</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="14" t="s">
-        <v>215</v>
+      <c r="A8" s="13" t="s">
+        <v>231</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>216</v>
+        <v>207</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>220</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
       </c>
+      <c r="K8" s="13" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="14"/>
+      <c r="A9" s="13"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
       <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.75">
+      <c r="C11" s="8"/>
+      <c r="D11" s="27"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="C13" s="8"/>
+      <c r="D13" s="26"/>
+    </row>
+    <row r="15" spans="1:11" ht="15.75">
+      <c r="C15" s="8"/>
+      <c r="D15" s="27"/>
+    </row>
+    <row r="20" spans="4:4">
+      <c r="D20" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="I2" r:id="rId3" display="QQQQQQQQQQQQQQQQQQQQ1@QQQQQQQQQQQQQQQQQQQQQQQQQQQQQQ"/>
-    <hyperlink ref="B8" r:id="rId4"/>
-    <hyperlink ref="D8" r:id="rId5"/>
-    <hyperlink ref="D5" r:id="rId6"/>
-    <hyperlink ref="D4" r:id="rId7"/>
-    <hyperlink ref="D3" r:id="rId8" display="navneet@gmail.com"/>
-    <hyperlink ref="D6" r:id="rId9"/>
-    <hyperlink ref="D7" r:id="rId10"/>
-    <hyperlink ref="D2" r:id="rId11"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="I2" r:id="rId2" display="QQQQQQQQQQQQQQQQQQQQ1@QQQQQQQQQQQQQQQQQQQQQQQQQQQQQQ"/>
+    <hyperlink ref="B8" r:id="rId3"/>
+    <hyperlink ref="D8" r:id="rId4"/>
+    <hyperlink ref="D5" r:id="rId5"/>
+    <hyperlink ref="D4" r:id="rId6"/>
+    <hyperlink ref="D6" r:id="rId7"/>
+    <hyperlink ref="D7" r:id="rId8"/>
+    <hyperlink ref="C4" r:id="rId9"/>
+    <hyperlink ref="C5" r:id="rId10"/>
+    <hyperlink ref="C6" r:id="rId11"/>
+    <hyperlink ref="D3" r:id="rId12"/>
+    <hyperlink ref="C3" r:id="rId13"/>
+    <hyperlink ref="D2" r:id="rId14"/>
+    <hyperlink ref="C2" r:id="rId15"/>
+    <hyperlink ref="C7" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId17"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1680,15 +2086,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D1:I2"/>
+  <dimension ref="D1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" customWidth="1"/>
+    <col min="7" max="7" width="30" customWidth="1"/>
     <col min="8" max="8" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1717,19 +2124,37 @@
       <c r="E2" t="s">
         <v>34</v>
       </c>
-      <c r="F2" t="s">
-        <v>12</v>
+      <c r="F2" s="13" t="s">
+        <v>218</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>216</v>
       </c>
       <c r="H2" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="4:9">
+      <c r="F4" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="G4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="4:9">
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G4" r:id="rId2"/>
+    <hyperlink ref="G5" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1744,8 +2169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H10" activeCellId="1" sqref="H2 H10"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1803,93 +2228,93 @@
         <v>25</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="T1" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="60" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2" s="5">
         <v>35291</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>56</v>
+      <c r="D2" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>209</v>
+        <v>36</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>206</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="M2" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="N2" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="O2" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="N2" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="O2" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>121</v>
+      <c r="P2" s="13" t="s">
+        <v>119</v>
       </c>
       <c r="Q2" s="11">
         <v>10</v>
       </c>
       <c r="R2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="S2" t="s">
-        <v>74</v>
-      </c>
-      <c r="T2" s="14" t="s">
-        <v>121</v>
+        <v>72</v>
+      </c>
+      <c r="T2" s="13" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -1904,169 +2329,169 @@
       <c r="I3" s="4"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
-      <c r="L3" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="M3" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="N3" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="O3" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="P3" s="20" t="s">
-        <v>111</v>
+      <c r="L3" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="N3" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="O3" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="P3" s="19" t="s">
+        <v>109</v>
       </c>
       <c r="Q3" s="11"/>
       <c r="R3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="S3" t="s">
-        <v>75</v>
-      </c>
-      <c r="T3" s="20" t="s">
-        <v>111</v>
+        <v>73</v>
+      </c>
+      <c r="T3" s="19" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:20">
-      <c r="L4" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="M4" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="N4" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="O4" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="P4" s="20" t="s">
-        <v>114</v>
+      <c r="L4" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="M4" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="N4" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="O4" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="P4" s="19" t="s">
+        <v>112</v>
       </c>
       <c r="Q4" s="11">
         <v>10</v>
       </c>
       <c r="R4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="S4" t="s">
-        <v>76</v>
-      </c>
-      <c r="T4" s="20" t="s">
-        <v>114</v>
+        <v>74</v>
+      </c>
+      <c r="T4" s="19" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:20">
-      <c r="L5" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="M5" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="N5" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="O5" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="P5" s="21" t="s">
-        <v>113</v>
+      <c r="L5" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="M5" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="N5" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="O5" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="P5" s="20" t="s">
+        <v>111</v>
       </c>
       <c r="Q5" s="11">
         <v>10</v>
       </c>
       <c r="R5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="S5" t="s">
-        <v>77</v>
-      </c>
-      <c r="T5" s="21" t="s">
-        <v>113</v>
+        <v>75</v>
+      </c>
+      <c r="T5" s="20" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:20">
-      <c r="L6" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="M6" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="N6" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="O6" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="P6" s="20" t="s">
-        <v>114</v>
+      <c r="L6" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="O6" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="P6" s="19" t="s">
+        <v>112</v>
       </c>
       <c r="Q6" s="11">
         <v>10</v>
       </c>
       <c r="R6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="S6" t="s">
-        <v>78</v>
-      </c>
-      <c r="T6" s="20" t="s">
-        <v>114</v>
+        <v>76</v>
+      </c>
+      <c r="T6" s="19" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:20">
-      <c r="L7" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="M7" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="N7" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="O7" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="P7" s="20" t="s">
-        <v>114</v>
+      <c r="L7" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="M7" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="O7" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="P7" s="19" t="s">
+        <v>112</v>
       </c>
       <c r="Q7" s="11">
         <v>10</v>
       </c>
       <c r="R7" t="s">
-        <v>72</v>
-      </c>
-      <c r="T7" s="20" t="s">
-        <v>114</v>
+        <v>70</v>
+      </c>
+      <c r="T7" s="19" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:20">
-      <c r="L8" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="M8" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="N8" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="O8" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="P8" s="20" t="s">
-        <v>114</v>
+      <c r="L8" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="N8" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="O8" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="P8" s="19" t="s">
+        <v>112</v>
       </c>
       <c r="Q8" s="11">
         <v>50</v>
       </c>
       <c r="R8" t="s">
-        <v>73</v>
-      </c>
-      <c r="T8" s="20" t="s">
-        <v>114</v>
+        <v>71</v>
+      </c>
+      <c r="T8" s="19" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2083,8 +2508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2128,16 +2553,16 @@
         <v>33</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="L1" t="s">
+        <v>154</v>
+      </c>
+      <c r="M1" t="s">
         <v>157</v>
-      </c>
-      <c r="M1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
@@ -2145,239 +2570,239 @@
         <v>28</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="D2" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" t="s">
+        <v>151</v>
+      </c>
+      <c r="L2" t="s">
         <v>153</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="G2" s="8" t="s">
+      <c r="M2" t="s">
         <v>158</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="I2" t="s">
-        <v>67</v>
-      </c>
-      <c r="J2" t="s">
-        <v>74</v>
-      </c>
-      <c r="K2" t="s">
-        <v>154</v>
-      </c>
-      <c r="L2" t="s">
-        <v>156</v>
-      </c>
-      <c r="M2" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="B3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>178</v>
+        <v>91</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>175</v>
       </c>
       <c r="E3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="B4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>153</v>
+        <v>92</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>150</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="M4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="B5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>153</v>
+        <v>93</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>150</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="M5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="B6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>153</v>
+        <v>94</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>150</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="B7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>153</v>
+        <v>149</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>150</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="B8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>153</v>
+        <v>149</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>150</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="C9" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>153</v>
+        <v>149</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>150</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="C10" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>153</v>
+        <v>149</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>150</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2394,10 +2819,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2406,126 +2831,506 @@
     <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="41.5703125" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" t="s">
+        <v>239</v>
+      </c>
+      <c r="F2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="D1" s="17"/>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="D3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" t="s">
+        <v>240</v>
+      </c>
+      <c r="F3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
         <v>74</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>92</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
         <v>81</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" t="s">
+        <v>241</v>
+      </c>
+      <c r="F4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="E5" t="s">
+        <v>242</v>
+      </c>
+      <c r="F5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
         <v>76</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>94</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
         <v>83</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D6" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="E6" t="s">
+        <v>243</v>
+      </c>
+      <c r="F6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7" t="s">
         <v>95</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C7" t="s">
         <v>84</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D7" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="E7" t="s">
+        <v>244</v>
+      </c>
+      <c r="F7" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" t="s">
         <v>96</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C8" t="s">
         <v>85</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="B7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="E8" t="s">
+        <v>245</v>
+      </c>
+      <c r="F8" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="C9" t="s">
         <v>86</v>
       </c>
-      <c r="D7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="B8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" t="s">
+        <v>246</v>
+      </c>
+      <c r="F9" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="C10" t="s">
         <v>87</v>
       </c>
-      <c r="D8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="C9" t="s">
+      <c r="E10" t="s">
+        <v>247</v>
+      </c>
+      <c r="F10" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="C11" t="s">
         <v>88</v>
       </c>
-      <c r="D9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="C10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="C11" t="s">
-        <v>90</v>
+      <c r="E11" t="s">
+        <v>248</v>
+      </c>
+      <c r="F11" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="E12" t="s">
+        <v>249</v>
+      </c>
+      <c r="F12" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="E13" t="s">
+        <v>250</v>
+      </c>
+      <c r="F13" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="E14" t="s">
+        <v>251</v>
+      </c>
+      <c r="F14" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="E15" t="s">
+        <v>252</v>
+      </c>
+      <c r="F15" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="E16" t="s">
+        <v>253</v>
+      </c>
+      <c r="F16" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6">
+      <c r="E17" t="s">
+        <v>254</v>
+      </c>
+      <c r="F17" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6">
+      <c r="E18" t="s">
+        <v>255</v>
+      </c>
+      <c r="F18" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="19" spans="5:6">
+      <c r="E19" t="s">
+        <v>256</v>
+      </c>
+      <c r="F19" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="20" spans="5:6">
+      <c r="E20" t="s">
+        <v>257</v>
+      </c>
+      <c r="F20" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="21" spans="5:6">
+      <c r="E21" t="s">
+        <v>258</v>
+      </c>
+      <c r="F21" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="22" spans="5:6">
+      <c r="E22" t="s">
+        <v>259</v>
+      </c>
+      <c r="F22" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="23" spans="5:6">
+      <c r="E23" t="s">
+        <v>260</v>
+      </c>
+      <c r="F23" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="24" spans="5:6">
+      <c r="E24" t="s">
+        <v>261</v>
+      </c>
+      <c r="F24" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="25" spans="5:6">
+      <c r="E25" t="s">
+        <v>262</v>
+      </c>
+      <c r="F25" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="26" spans="5:6">
+      <c r="E26" t="s">
+        <v>263</v>
+      </c>
+      <c r="F26" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="27" spans="5:6">
+      <c r="E27" t="s">
+        <v>264</v>
+      </c>
+      <c r="F27" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="28" spans="5:6">
+      <c r="E28" t="s">
+        <v>265</v>
+      </c>
+      <c r="F28" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="29" spans="5:6">
+      <c r="E29" t="s">
+        <v>266</v>
+      </c>
+      <c r="F29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="30" spans="5:6">
+      <c r="E30" t="s">
+        <v>267</v>
+      </c>
+      <c r="F30" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="31" spans="5:6">
+      <c r="E31" t="s">
+        <v>268</v>
+      </c>
+      <c r="F31" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="32" spans="5:6">
+      <c r="E32" t="s">
+        <v>269</v>
+      </c>
+      <c r="F32" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6">
+      <c r="E33" t="s">
+        <v>270</v>
+      </c>
+      <c r="F33" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6">
+      <c r="E34" t="s">
+        <v>271</v>
+      </c>
+      <c r="F34" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6">
+      <c r="E35" t="s">
+        <v>272</v>
+      </c>
+      <c r="F35" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6">
+      <c r="E36" t="s">
+        <v>273</v>
+      </c>
+      <c r="F36" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6">
+      <c r="E37" t="s">
+        <v>274</v>
+      </c>
+      <c r="F37" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6">
+      <c r="E38" t="s">
+        <v>275</v>
+      </c>
+      <c r="F38" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6">
+      <c r="E39" t="s">
+        <v>276</v>
+      </c>
+      <c r="F39" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6">
+      <c r="E40" t="s">
+        <v>277</v>
+      </c>
+      <c r="F40" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="41" spans="5:6">
+      <c r="E41" t="s">
+        <v>278</v>
+      </c>
+      <c r="F41" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="42" spans="5:6">
+      <c r="E42" t="s">
+        <v>279</v>
+      </c>
+      <c r="F42" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6">
+      <c r="E43" t="s">
+        <v>280</v>
+      </c>
+      <c r="F43" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6">
+      <c r="E44" t="s">
+        <v>281</v>
+      </c>
+      <c r="F44" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6">
+      <c r="E45" t="s">
+        <v>282</v>
+      </c>
+      <c r="F45" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6">
+      <c r="E46" t="s">
+        <v>283</v>
+      </c>
+      <c r="F46" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6">
+      <c r="E47" t="s">
+        <v>284</v>
+      </c>
+      <c r="F47" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6">
+      <c r="E48" t="s">
+        <v>285</v>
+      </c>
+      <c r="F48" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="49" spans="5:6">
+      <c r="E49" t="s">
+        <v>286</v>
+      </c>
+      <c r="F49" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="50" spans="5:6">
+      <c r="E50" t="s">
+        <v>287</v>
+      </c>
+      <c r="F50" t="s">
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -2538,7 +3343,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2560,107 +3365,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="F1" s="22" t="s">
+      <c r="E4" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="G1" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2687,37 +3500,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>135</v>
+      <c r="D1" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="2:6">
-      <c r="B2" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>134</v>
+      <c r="B2" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2730,7 +3543,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" activeCellId="1" sqref="G2 G17"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2742,155 +3555,155 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="E1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="B2" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="21" t="s">
+      <c r="D2" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>55</v>
+      <c r="E3" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>54</v>
+      <c r="A4" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="G5" s="21" t="s">
-        <v>106</v>
+      <c r="A5" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>54</v>
+      <c r="A6" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="20"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="19"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="11"/>
-      <c r="H8" s="20"/>
+      <c r="H8" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updation in Saving Advantage Plan and SmartTermPlan
</commit_message>
<xml_diff>
--- a/src/test/resources/MasterData.xlsx
+++ b/src/test/resources/MasterData.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mpro\mpro-automation\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="743" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="743" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="365">
   <si>
     <t>username</t>
   </si>
@@ -1136,12 +1141,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy"/>
     <numFmt numFmtId="165" formatCode="\1\2\3\4\5\6\7\8\90\9\8\7\6\5\4\3\2\2\1\2\3\4\5\6\7\8\90\9\8\7\6\5"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1314,6 +1319,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1360,7 +1373,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1392,9 +1405,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1426,6 +1440,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1601,21 +1616,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.28515625" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="1025" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1623,7 +1638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>100121</v>
       </c>
@@ -1631,7 +1646,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>585529</v>
       </c>
@@ -1639,7 +1654,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1657,14 +1672,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="28.85546875" customWidth="1"/>
@@ -1679,7 +1694,7 @@
     <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="45">
+    <row r="1" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>176</v>
       </c>
@@ -1720,7 +1735,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="195">
+    <row r="2" spans="1:13" ht="195" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>177</v>
       </c>
@@ -1758,7 +1773,7 @@
         <v>1234567</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
       <c r="B3" s="24"/>
       <c r="C3" s="24" t="s">
@@ -1789,7 +1804,7 @@
         <v>12345678</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
       <c r="B4" s="24"/>
       <c r="C4" s="24" t="s">
@@ -1817,7 +1832,7 @@
         <v>12345678910111</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="24"/>
       <c r="B5" s="24"/>
       <c r="C5" s="24" t="s">
@@ -1845,7 +1860,7 @@
         <v>123456789101112</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="24"/>
       <c r="C6" s="24" t="s">
@@ -1873,7 +1888,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
       <c r="B7" s="24"/>
       <c r="C7" s="24"/>
@@ -1897,7 +1912,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
       <c r="B8" s="24"/>
       <c r="C8" s="24"/>
@@ -1915,7 +1930,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
@@ -1929,7 +1944,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>
@@ -1943,7 +1958,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="24"/>
       <c r="C11" s="24"/>
@@ -1966,26 +1981,26 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
@@ -2000,7 +2015,7 @@
     <col min="12" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="45">
+    <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -2035,7 +2050,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75">
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>233</v>
       </c>
@@ -2070,7 +2085,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>228</v>
       </c>
@@ -2089,7 +2104,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>229</v>
       </c>
@@ -2111,7 +2126,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>230</v>
       </c>
@@ -2133,7 +2148,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>231</v>
       </c>
@@ -2155,7 +2170,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>232</v>
       </c>
@@ -2175,7 +2190,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>227</v>
       </c>
@@ -2192,7 +2207,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="C9" s="8"/>
       <c r="D9" s="28" t="s">
@@ -2200,7 +2215,7 @@
       </c>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C10" s="8">
         <v>9873970332</v>
       </c>
@@ -2208,25 +2223,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75">
+    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C11" s="8"/>
       <c r="D11" s="27" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75">
+    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D12" s="27" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C13" s="8"/>
       <c r="D13" s="26"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75">
+    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D15" s="27"/>
     </row>
-    <row r="20" spans="4:4">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="8"/>
     </row>
   </sheetData>
@@ -2258,14 +2273,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="30.28515625" customWidth="1"/>
     <col min="5" max="5" width="20.42578125" customWidth="1"/>
@@ -2274,7 +2289,7 @@
     <col min="8" max="8" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:8">
+    <row r="1" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
@@ -2291,7 +2306,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="4:8">
+    <row r="2" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>11</v>
       </c>
@@ -2308,7 +2323,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="4:8">
+    <row r="4" spans="4:8" x14ac:dyDescent="0.25">
       <c r="F4" s="13" t="s">
         <v>217</v>
       </c>
@@ -2316,7 +2331,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="4:8">
+    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>12</v>
       </c>
@@ -2324,7 +2339,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="4:8">
+    <row r="10" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>363</v>
       </c>
@@ -2335,7 +2350,7 @@
         <v>33654</v>
       </c>
     </row>
-    <row r="11" spans="4:8">
+    <row r="11" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>364</v>
       </c>
@@ -2356,14 +2371,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="58.42578125" customWidth="1"/>
@@ -2383,7 +2398,7 @@
     <col min="20" max="20" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2445,7 +2460,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="60" customHeight="1">
+    <row r="2" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>201</v>
       </c>
@@ -2507,7 +2522,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>360</v>
       </c>
@@ -2553,7 +2568,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="L4" s="19" t="s">
         <v>52</v>
       </c>
@@ -2582,7 +2597,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="L5" s="20" t="s">
         <v>104</v>
       </c>
@@ -2611,7 +2626,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="L6" s="19" t="s">
         <v>52</v>
       </c>
@@ -2640,7 +2655,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="L7" s="19" t="s">
         <v>52</v>
       </c>
@@ -2666,7 +2681,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="L8" s="19" t="s">
         <v>52</v>
       </c>
@@ -2703,14 +2718,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="94.140625" customWidth="1"/>
     <col min="2" max="2" width="88.42578125" customWidth="1"/>
@@ -2728,7 +2743,7 @@
     <col min="14" max="14" width="39.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -2766,7 +2781,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" customHeight="1">
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
@@ -2810,7 +2825,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>91</v>
       </c>
@@ -2842,7 +2857,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>92</v>
       </c>
@@ -2871,7 +2886,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>93</v>
       </c>
@@ -2900,7 +2915,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>94</v>
       </c>
@@ -2929,7 +2944,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>95</v>
       </c>
@@ -2952,7 +2967,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>96</v>
       </c>
@@ -2975,7 +2990,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C9" s="8" t="s">
         <v>149</v>
       </c>
@@ -2992,7 +3007,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C10" s="8" t="s">
         <v>149</v>
       </c>
@@ -3022,14 +3037,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
@@ -3040,7 +3055,7 @@
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>78</v>
       </c>
@@ -3062,7 +3077,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -3088,7 +3103,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -3114,7 +3129,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -3140,7 +3155,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -3166,7 +3181,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -3189,7 +3204,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>95</v>
       </c>
@@ -3209,7 +3224,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>96</v>
       </c>
@@ -3229,7 +3244,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>86</v>
       </c>
@@ -3246,7 +3261,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>87</v>
       </c>
@@ -3260,7 +3275,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>88</v>
       </c>
@@ -3274,7 +3289,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>245</v>
       </c>
@@ -3282,7 +3297,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>246</v>
       </c>
@@ -3290,7 +3305,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
         <v>247</v>
       </c>
@@ -3298,7 +3313,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>248</v>
       </c>
@@ -3306,7 +3321,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>249</v>
       </c>
@@ -3314,7 +3329,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="17" spans="5:6">
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
         <v>250</v>
       </c>
@@ -3322,7 +3337,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="18" spans="5:6">
+    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
         <v>251</v>
       </c>
@@ -3330,7 +3345,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="19" spans="5:6">
+    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
         <v>252</v>
       </c>
@@ -3338,7 +3353,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="20" spans="5:6">
+    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>253</v>
       </c>
@@ -3346,7 +3361,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="21" spans="5:6">
+    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>254</v>
       </c>
@@ -3354,7 +3369,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="22" spans="5:6">
+    <row r="22" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
         <v>255</v>
       </c>
@@ -3362,7 +3377,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="23" spans="5:6">
+    <row r="23" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>256</v>
       </c>
@@ -3370,7 +3385,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="24" spans="5:6">
+    <row r="24" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>257</v>
       </c>
@@ -3378,7 +3393,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="25" spans="5:6">
+    <row r="25" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
         <v>258</v>
       </c>
@@ -3386,7 +3401,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="26" spans="5:6">
+    <row r="26" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
         <v>259</v>
       </c>
@@ -3394,7 +3409,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="27" spans="5:6">
+    <row r="27" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
         <v>260</v>
       </c>
@@ -3402,7 +3417,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="28" spans="5:6">
+    <row r="28" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
         <v>261</v>
       </c>
@@ -3410,7 +3425,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="29" spans="5:6">
+    <row r="29" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
         <v>262</v>
       </c>
@@ -3418,7 +3433,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="30" spans="5:6">
+    <row r="30" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
         <v>263</v>
       </c>
@@ -3426,7 +3441,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="31" spans="5:6">
+    <row r="31" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
         <v>264</v>
       </c>
@@ -3434,7 +3449,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="32" spans="5:6">
+    <row r="32" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
         <v>265</v>
       </c>
@@ -3442,7 +3457,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="33" spans="5:6">
+    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
         <v>266</v>
       </c>
@@ -3450,7 +3465,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="34" spans="5:6">
+    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
         <v>267</v>
       </c>
@@ -3458,7 +3473,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="35" spans="5:6">
+    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
         <v>268</v>
       </c>
@@ -3466,7 +3481,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="36" spans="5:6">
+    <row r="36" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
         <v>269</v>
       </c>
@@ -3474,7 +3489,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="37" spans="5:6">
+    <row r="37" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
         <v>270</v>
       </c>
@@ -3482,7 +3497,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="38" spans="5:6">
+    <row r="38" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
         <v>271</v>
       </c>
@@ -3490,7 +3505,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="39" spans="5:6">
+    <row r="39" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
         <v>272</v>
       </c>
@@ -3498,7 +3513,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="40" spans="5:6">
+    <row r="40" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
         <v>273</v>
       </c>
@@ -3506,7 +3521,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="41" spans="5:6">
+    <row r="41" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
         <v>274</v>
       </c>
@@ -3514,7 +3529,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="42" spans="5:6">
+    <row r="42" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
         <v>275</v>
       </c>
@@ -3522,7 +3537,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="43" spans="5:6">
+    <row r="43" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
         <v>276</v>
       </c>
@@ -3530,7 +3545,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="44" spans="5:6">
+    <row r="44" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
         <v>277</v>
       </c>
@@ -3538,7 +3553,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="45" spans="5:6">
+    <row r="45" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
         <v>278</v>
       </c>
@@ -3546,7 +3561,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="46" spans="5:6">
+    <row r="46" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E46" t="s">
         <v>279</v>
       </c>
@@ -3554,7 +3569,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="47" spans="5:6">
+    <row r="47" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E47" t="s">
         <v>280</v>
       </c>
@@ -3562,7 +3577,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="48" spans="5:6">
+    <row r="48" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E48" t="s">
         <v>281</v>
       </c>
@@ -3570,7 +3585,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="49" spans="5:6">
+    <row r="49" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E49" t="s">
         <v>282</v>
       </c>
@@ -3578,7 +3593,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="50" spans="5:6">
+    <row r="50" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E50" t="s">
         <v>283</v>
       </c>
@@ -3590,14 +3605,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="65.7109375" customWidth="1"/>
     <col min="2" max="2" width="34.28515625" customWidth="1"/>
@@ -3615,7 +3630,7 @@
     <col min="16" max="16" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>118</v>
       </c>
@@ -3649,7 +3664,7 @@
       <c r="O1" s="21"/>
       <c r="P1" s="21"/>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>134</v>
       </c>
@@ -3678,7 +3693,7 @@
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>135</v>
       </c>
@@ -3707,7 +3722,7 @@
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>136</v>
       </c>
@@ -3734,14 +3749,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="69.7109375" customWidth="1"/>
     <col min="2" max="2" width="55" customWidth="1"/>
@@ -3752,7 +3767,7 @@
     <col min="7" max="8" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1" s="21" t="s">
         <v>129</v>
       </c>
@@ -3769,7 +3784,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="s">
         <v>130</v>
       </c>
@@ -3792,21 +3807,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26:E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
     <col min="7" max="7" width="25.5703125" customWidth="1"/>
     <col min="8" max="8" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>137</v>
       </c>
@@ -3828,8 +3843,11 @@
       <c r="G1" s="4" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="H1" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>144</v>
       </c>
@@ -3851,8 +3869,11 @@
       <c r="G2" s="20" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="H2">
+        <v>230000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>144</v>
       </c>
@@ -3875,7 +3896,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>144</v>
       </c>
@@ -3898,7 +3919,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>144</v>
       </c>
@@ -3921,7 +3942,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>144</v>
       </c>
@@ -3944,7 +3965,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -3954,7 +3975,7 @@
       <c r="G7" s="20"/>
       <c r="H7" s="19"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="H8" s="19"/>
     </row>

</xml_diff>

<commit_message>
Shiksha Plus Super Plan By Systematic Transfer Plan Case
</commit_message>
<xml_diff>
--- a/src/test/resources/MasterData.xlsx
+++ b/src/test/resources/MasterData.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mpro\mpro-automation\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="743" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14535" windowHeight="2745" tabRatio="743" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,8 @@
     <sheet name="personalDetailsSectionValid" sheetId="10" r:id="rId10"/>
     <sheet name="Sheet1" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <oleSize ref="B1:D7"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -34,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="366">
   <si>
     <t>username</t>
   </si>
@@ -1136,6 +1132,9 @@
   </si>
   <si>
     <t>Ramalingeshwarao maddala</t>
+  </si>
+  <si>
+    <t>Adam Gill</t>
   </si>
 </sst>
 </file>
@@ -2719,10 +2718,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2743,7 +2742,7 @@
     <col min="14" max="14" width="39.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -2781,7 +2780,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
@@ -2824,8 +2823,11 @@
       <c r="N2" s="31" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>91</v>
       </c>
@@ -2857,7 +2859,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>92</v>
       </c>
@@ -2886,7 +2888,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>93</v>
       </c>
@@ -2915,7 +2917,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>94</v>
       </c>
@@ -2944,7 +2946,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>95</v>
       </c>
@@ -2967,7 +2969,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>96</v>
       </c>
@@ -2990,7 +2992,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C9" s="8" t="s">
         <v>149</v>
       </c>
@@ -3007,7 +3009,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C10" s="8" t="s">
         <v>149</v>
       </c>
@@ -3810,7 +3812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated Shiksha Plus Super Plan
</commit_message>
<xml_diff>
--- a/src/test/resources/MasterData.xlsx
+++ b/src/test/resources/MasterData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14535" windowHeight="2745" tabRatio="743" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13905" windowHeight="3855" tabRatio="743" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Sheet1" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <oleSize ref="B1:D7"/>
+  <oleSize ref="A6:E13"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -1113,12 +1113,6 @@
     <t>InternationalPhoneValidation</t>
   </si>
   <si>
-    <t>mprotest4@gmail.com</t>
-  </si>
-  <si>
-    <t>qwerty@123</t>
-  </si>
-  <si>
     <t>suniti</t>
   </si>
   <si>
@@ -1135,6 +1129,13 @@
   </si>
   <si>
     <t>Adam Gill</t>
+  </si>
+  <si>
+    <t>pmaxlife071@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+pmaxlife071@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1242,7 +1243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1311,6 +1312,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1995,8 +1999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2049,7 +2053,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>233</v>
       </c>
@@ -2059,8 +2063,8 @@
       <c r="C2" s="13" t="s">
         <v>333</v>
       </c>
-      <c r="D2" s="27" t="s">
-        <v>358</v>
+      <c r="D2" s="34" t="s">
+        <v>365</v>
       </c>
       <c r="E2">
         <v>98760987123</v>
@@ -2222,15 +2226,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C11" s="8"/>
-      <c r="D11" s="27" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D12" s="27" t="s">
-        <v>359</v>
+      <c r="D11" s="8" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D12" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2261,9 +2265,11 @@
     <hyperlink ref="C10" r:id="rId14" display="8374848595@"/>
     <hyperlink ref="C7" r:id="rId15"/>
     <hyperlink ref="D10" r:id="rId16"/>
+    <hyperlink ref="D11" r:id="rId17"/>
+    <hyperlink ref="D12" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId17"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId19"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2340,10 +2346,10 @@
     </row>
     <row r="10" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E10" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F10" s="33">
         <v>33654</v>
@@ -2351,7 +2357,7 @@
     </row>
     <row r="11" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -2523,10 +2529,10 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="4"/>
@@ -2720,7 +2726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
@@ -2824,7 +2830,7 @@
         <v>355</v>
       </c>
       <c r="P2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Created New Plan MaxLife Life Perfect Partner Super Test
</commit_message>
<xml_diff>
--- a/src/test/resources/MasterData.xlsx
+++ b/src/test/resources/MasterData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13905" windowHeight="3855" tabRatio="743" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12915" windowHeight="2430" tabRatio="743" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Sheet1" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <oleSize ref="A6:E13"/>
+  <oleSize ref="A6:E11"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="367">
   <si>
     <t>username</t>
   </si>
@@ -1136,6 +1136,9 @@
   <si>
     <t xml:space="preserve">
 pmaxlife071@gmail.com</t>
+  </si>
+  <si>
+    <t>Ammount</t>
   </si>
 </sst>
 </file>
@@ -1997,10 +2000,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2018,7 +2021,7 @@
     <col min="12" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -2052,8 +2055,11 @@
       <c r="K1" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="L1" s="3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>233</v>
       </c>
@@ -2087,8 +2093,11 @@
       <c r="K2" s="13" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>228</v>
       </c>
@@ -2107,7 +2116,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>229</v>
       </c>
@@ -2129,7 +2138,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>230</v>
       </c>
@@ -2151,7 +2160,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>231</v>
       </c>
@@ -2173,7 +2182,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>232</v>
       </c>
@@ -2193,7 +2202,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>227</v>
       </c>
@@ -2210,7 +2219,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="C9" s="8"/>
       <c r="D9" s="28" t="s">
@@ -2218,7 +2227,7 @@
       </c>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" s="8">
         <v>9873970332</v>
       </c>
@@ -2226,22 +2235,22 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" s="8"/>
       <c r="D11" s="8" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D12" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C13" s="8"/>
       <c r="D13" s="26"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D15" s="27"/>
     </row>
     <row r="20" spans="4:4" x14ac:dyDescent="0.25">

</xml_diff>